<commit_message>
Latest in progress commit:
    * Add Plugin support for AssertionProviders, TestProviders and DataProviders using the ServiceLoader framework.
    * Added a Context and Config object (not in use yet).
    * Major refactoring (still a lot to do)
</commit_message>
<xml_diff>
--- a/lambda-core/src/main/resources/tests.xlsx
+++ b/lambda-core/src/main/resources/tests.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
   <si>
     <t>testWebDriver</t>
   </si>
@@ -60,9 +60,6 @@
     <t>open</t>
   </si>
   <si>
-    <t>/</t>
-  </si>
-  <si>
     <t>click</t>
   </si>
   <si>
@@ -124,13 +121,16 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>/domainname/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -158,6 +158,12 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -645,10 +651,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D18"/>
+  <dimension ref="A2:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -664,13 +670,13 @@
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -678,39 +684,39 @@
         <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="4">
         <v>10</v>
@@ -718,78 +724,14 @@
     </row>
     <row r="8" spans="1:4">
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="B15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="B16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3">
-      <c r="B17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3">
-      <c r="B18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -804,7 +746,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -831,34 +773,34 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
         <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
         <v>27</v>
-      </c>
-      <c r="B6" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -903,34 +845,34 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
         <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
         <v>27</v>
-      </c>
-      <c r="B6" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Added Spring support to the CLI interface to Inject dependencies into Lambda and Test cases - Removing TestNG runner from Lambda in favour of a basic test runner executed within Lambda (allows Spring injection. Potentiall look at creating a TestNG -> spring bridge similar to AbstractTestNGSpringContextTests) - Fixed bugs with DataProviders in JavassistTestBuilderImpl - Added plugin support for all provider types - Basic Context lifecycle support for plugins
</commit_message>
<xml_diff>
--- a/lambda-core/src/main/resources/tests.xlsx
+++ b/lambda-core/src/main/resources/tests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2940" yWindow="240" windowWidth="33600" windowHeight="20480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
   <si>
     <t>testWebDriver</t>
   </si>
@@ -54,42 +54,15 @@
     <t>password</t>
   </si>
   <si>
-    <t>testRetailHomepage</t>
-  </si>
-  <si>
     <t>open</t>
   </si>
   <si>
-    <t>click</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>thisisadomainname</t>
   </si>
   <si>
-    <t>assertTextPresent</t>
-  </si>
-  <si>
-    <t>waitForPageToLoad</t>
-  </si>
-  <si>
     <t>thisisadomainname.com.au</t>
   </si>
   <si>
-    <t>id=$searchBox</t>
-  </si>
-  <si>
-    <t>id=$searchButton</t>
-  </si>
-  <si>
-    <t>$domainSearch</t>
-  </si>
-  <si>
-    <t>$domainName is available</t>
-  </si>
-  <si>
     <t>domainName</t>
   </si>
   <si>
@@ -123,7 +96,22 @@
     <t>Value</t>
   </si>
   <si>
-    <t>/domainname/</t>
+    <t>matt</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>domain</t>
+  </si>
+  <si>
+    <t>testEmailServices</t>
+  </si>
+  <si>
+    <t>/email-services/</t>
+  </si>
+  <si>
+    <t>email</t>
   </si>
 </sst>
 </file>
@@ -186,8 +174,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -214,17 +212,27 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -651,10 +659,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D8"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection sqref="A1:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -665,74 +673,43 @@
     <col min="4" max="4" width="13.83203125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>32</v>
+      <c r="C2" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="B3" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="C6" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -743,10 +720,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -773,38 +750,47 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
         <v>26</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -815,10 +801,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -845,34 +831,42 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
         <v>26</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WIP commit for machine migration
</commit_message>
<xml_diff>
--- a/lambda-core/src/main/resources/tests.xlsx
+++ b/lambda-core/src/main/resources/tests.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="43">
   <si>
     <t>testWebDriver</t>
   </si>
@@ -54,15 +54,42 @@
     <t>password</t>
   </si>
   <si>
+    <t>testRetailHomepage</t>
+  </si>
+  <si>
     <t>open</t>
   </si>
   <si>
+    <t>click</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
     <t>thisisadomainname</t>
   </si>
   <si>
+    <t>assertTextPresent</t>
+  </si>
+  <si>
+    <t>waitForPageToLoad</t>
+  </si>
+  <si>
     <t>thisisadomainname.com.au</t>
   </si>
   <si>
+    <t>id=$searchBox</t>
+  </si>
+  <si>
+    <t>id=$searchButton</t>
+  </si>
+  <si>
+    <t>$domainSearch</t>
+  </si>
+  <si>
+    <t>$domainName is available</t>
+  </si>
+  <si>
     <t>domainName</t>
   </si>
   <si>
@@ -96,13 +123,25 @@
     <t>Value</t>
   </si>
   <si>
+    <t>/domainname/</t>
+  </si>
+  <si>
     <t>matt</t>
   </si>
   <si>
+    <t>$message</t>
+  </si>
+  <si>
     <t>message</t>
   </si>
   <si>
     <t>domain</t>
+  </si>
+  <si>
+    <t>testFoo</t>
+  </si>
+  <si>
+    <t>/</t>
   </si>
   <si>
     <t>testEmailServices</t>
@@ -659,7 +698,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A2:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD13"/>
@@ -673,38 +712,133 @@
     <col min="4" max="4" width="13.83203125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
     <row r="2" spans="1:4">
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>28</v>
+      <c r="A2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="B3" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>29</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="C6" s="4"/>
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3">
+      <c r="C19" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -750,42 +884,42 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
         <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -831,42 +965,42 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>